<commit_message>
fix compile for XLUtils
</commit_message>
<xml_diff>
--- a/KD_java/src/dataEngine/DataEngine.xlsx
+++ b/KD_java/src/dataEngine/DataEngine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taracz\KD_java\KD_java\bin\dataEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taracz\KD_java\KD_java\src\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E928EE9-B4B2-4FB2-B31E-3EAF1B095AEF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B815ED8-B21D-4F4F-BBFF-39B8677F6657}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4305" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{756D6F96-C56C-46A1-AAEF-29B37443CBE0}"/>
+    <workbookView xWindow="-28920" yWindow="-4305" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{756D6F96-C56C-46A1-AAEF-29B37443CBE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -691,9 +691,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9689450B-F3D8-41A8-A088-754F0670C56F}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,9 +750,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4D8A81-4F74-403D-8139-B40670DEAF6E}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,6 +802,9 @@
       <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
@@ -818,6 +821,9 @@
       </c>
       <c r="C3" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>25</v>

</xml_diff>